<commit_message>
performance tests for QUERY function are added
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it-performance/src/test/resources/datamodel/query/QUERY_1000set_1000times.xlsx
+++ b/calculation-engine/engine-tests/engine-it-performance/src/test/resources/datamodel/query/QUERY_1000set_1000times.xlsx
@@ -4,17 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1005" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="1455" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -357,23 +353,23 @@
   <dimension ref="A1:A1000"/>
   <sheetViews>
     <sheetView showFormulas="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="e">
-        <f ca="1">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f ca="1">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="e">
-        <f t="shared" ref="A2:A65" ca="1" si="0">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A2:A65" ca="1" si="0">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -757,7 +753,7 @@
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="e">
-        <f t="shared" ref="A66:A129" ca="1" si="1">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A66:A129" ca="1" si="1">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -1141,7 +1137,7 @@
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="e">
-        <f t="shared" ref="A130:A193" ca="1" si="2">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A130:A193" ca="1" si="2">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -1525,7 +1521,7 @@
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A194" t="e">
-        <f t="shared" ref="A194:A257" ca="1" si="3">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A194:A257" ca="1" si="3">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -1909,7 +1905,7 @@
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A258" t="e">
-        <f t="shared" ref="A258:A321" ca="1" si="4">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A258:A321" ca="1" si="4">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -2293,7 +2289,7 @@
     </row>
     <row r="322" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A322" t="e">
-        <f t="shared" ref="A322:A385" ca="1" si="5">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A322:A385" ca="1" si="5">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -2677,7 +2673,7 @@
     </row>
     <row r="386" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A386" t="e">
-        <f t="shared" ref="A386:A449" ca="1" si="6">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A386:A449" ca="1" si="6">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -3061,7 +3057,7 @@
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A450" t="e">
-        <f t="shared" ref="A450:A513" ca="1" si="7">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A450:A513" ca="1" si="7">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -3445,7 +3441,7 @@
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A514" t="e">
-        <f t="shared" ref="A514:A577" ca="1" si="8">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A514:A577" ca="1" si="8">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -3829,7 +3825,7 @@
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A578" t="e">
-        <f t="shared" ref="A578:A641" ca="1" si="9">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A578:A641" ca="1" si="9">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -4213,7 +4209,7 @@
     </row>
     <row r="642" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A642" t="e">
-        <f t="shared" ref="A642:A705" ca="1" si="10">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A642:A705" ca="1" si="10">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -4597,7 +4593,7 @@
     </row>
     <row r="706" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A706" t="e">
-        <f t="shared" ref="A706:A769" ca="1" si="11">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A706:A769" ca="1" si="11">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -4981,7 +4977,7 @@
     </row>
     <row r="770" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A770" t="e">
-        <f t="shared" ref="A770:A833" ca="1" si="12">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A770:A833" ca="1" si="12">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -5365,7 +5361,7 @@
     </row>
     <row r="834" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A834" t="e">
-        <f t="shared" ref="A834:A897" ca="1" si="13">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A834:A897" ca="1" si="13">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -5749,7 +5745,7 @@
     </row>
     <row r="898" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A898" t="e">
-        <f t="shared" ref="A898:A961" ca="1" si="14">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A898:A961" ca="1" si="14">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>
@@ -6133,7 +6129,7 @@
     </row>
     <row r="962" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A962" t="e">
-        <f t="shared" ref="A962:A1000" ca="1" si="15">QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local")</f>
+        <f t="shared" ref="A962:A1000" ca="1" si="15">INDEX(QUERY("ShuffledDataSet1000","ShuffledDataSet1000_1000_local"),1,1)</f>
         <v>#NAME?</v>
       </c>
     </row>

</xml_diff>